<commit_message>
Update exported sheet workbooks
</commit_message>
<xml_diff>
--- a/data/sheets/Aluminium.xlsx
+++ b/data/sheets/Aluminium.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28aa9e46087b5738/0-Concordia_Capital/excel_to_https/excel_web_refresh/export/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AEC5B9D-8315-46CD-91E6-D87991C058FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A506CFDA-DF9E-4F2E-B955-D23C4B29B902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C28C00B-4F42-4383-A5BE-67525245BE31}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EE4D278-9D82-4981-81BA-9A2EAB7E5F12}"/>
   </bookViews>
   <sheets>
-    <sheet name="Aluminium" sheetId="2" r:id="rId1"/>
+    <sheet name="Aluminium" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -48,7 +48,6 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_MONTH">15000</definedName>
     <definedName name="IQ_MTD" hidden="1">800000</definedName>
-    <definedName name="IQ_NAMES_REVISION_DATE_" localSheetId="0" hidden="1">46064.7990046296</definedName>
     <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">46064.7990046296</definedName>
     <definedName name="IQ_NTM">6000</definedName>
     <definedName name="IQ_QTD" hidden="1">750000</definedName>
@@ -291,14 +290,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -604,213 +596,211 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="5" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1" xr:uid="{61946C0B-6A81-4474-8ABF-7BAB0EF9D442}"/>
-    <cellStyle name="百分比 2" xfId="2" xr:uid="{8FB4E9C9-2BD9-46C8-B80B-40268E0EB5A4}"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1288,7 +1278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940BF989-DC1A-4650-AF7E-C1FB5FC905DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AB0F99-61EF-4223-AF83-8FE08BAFF933}">
   <dimension ref="A1:AB50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -1299,7 +1289,7 @@
       <selection pane="bottomRight" activeCell="I2678" sqref="I2678"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="5" width="12.77734375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -1323,7 +1313,7 @@
     <col min="26" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1435,7 +1425,7 @@
       <c r="Y2" s="17"/>
       <c r="AB2" s="18"/>
     </row>
-    <row r="3" spans="1:28" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
@@ -1477,7 +1467,7 @@
       </c>
       <c r="AB3" s="25"/>
     </row>
-    <row r="4" spans="1:28" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="13.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J4" s="12"/>
       <c r="K4" s="19"/>
       <c r="L4" s="21"/>
@@ -1493,7 +1483,7 @@
       <c r="Y4" s="25"/>
       <c r="AB4" s="25"/>
     </row>
-    <row r="5" spans="1:28" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="16.8" x14ac:dyDescent="0.25">
       <c r="H5" s="27" t="s">
         <v>35</v>
       </c>
@@ -1516,7 +1506,7 @@
       <c r="Y5" s="31"/>
       <c r="AB5" s="25"/>
     </row>
-    <row r="6" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J6, A$3)</f>
         <v>#NAME?</v>
@@ -1616,7 +1606,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J7, A$3)</f>
         <v>#NAME?</v>
@@ -1704,7 +1694,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J8, A$3)</f>
         <v>#NAME?</v>
@@ -1792,7 +1782,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J9, A$3)</f>
         <v>#NAME?</v>
@@ -1975,7 +1965,7 @@
       <c r="Y11" s="31"/>
       <c r="AB11" s="25"/>
     </row>
-    <row r="12" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J12, A$3)</f>
         <v>#NAME?</v>
@@ -2063,7 +2053,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J13, A$3)</f>
         <v>#NAME?</v>
@@ -2151,7 +2141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="e">
         <f ca="1">_xll.SNL.Clients.Office.Excel.Functions.SPG($J14, A$3)</f>
         <v>#NAME?</v>
@@ -2537,7 +2527,7 @@
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="65"/>
       <c r="B50" s="65"/>
       <c r="C50" s="65"/>

</xml_diff>